<commit_message>
finished BLASTING for next closest assignment for unassigned species in 12s
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
+++ b/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{1427330D-7909-4C12-9002-F163BFB2FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F99513-849F-4BC6-8412-191BB61AB17A}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{1427330D-7909-4C12-9002-F163BFB2FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CDD658-C83B-4558-8F2B-E25E99E68E8C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5928" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5956" uniqueCount="504">
   <si>
     <t>Sequence</t>
   </si>
@@ -9457,6 +9457,15 @@
   </si>
   <si>
     <t>99.36% Lumpenella longirostris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98.09% Xenolumpenus longipterus, Poroclinus rothrocki, </t>
+  </si>
+  <si>
+    <t>99.37% Oncorhynchus kawamurae, Oncorhynchus nerka</t>
+  </si>
+  <si>
+    <t>99.36% Onchorhynchus nerka</t>
   </si>
 </sst>
 </file>
@@ -9979,8 +9988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I256" sqref="I256"/>
+    <sheetView topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="A293" sqref="A293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22155,8 +22164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BCACDE-7C62-4795-BCF1-A029DECBB41A}">
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J160" sqref="J160"/>
+    <sheetView topLeftCell="A111" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26528,8 +26537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5085614D-A8E1-47C2-8EAC-787C4920C226}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28708,6 +28717,9 @@
       <c r="J83" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="L83" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -28734,6 +28746,9 @@
       <c r="J84" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="L84" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -28760,6 +28775,9 @@
       <c r="J85" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="L85" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -28789,6 +28807,9 @@
       <c r="J86" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="L86" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -28818,6 +28839,9 @@
       <c r="J87" s="3" t="s">
         <v>352</v>
       </c>
+      <c r="L87" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -28844,6 +28868,9 @@
       <c r="J88" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L88" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -28870,6 +28897,9 @@
       <c r="J89" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L89" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
@@ -28896,6 +28926,9 @@
       <c r="J90" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L90" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
@@ -28922,6 +28955,9 @@
       <c r="J91" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L91" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -28948,6 +28984,9 @@
       <c r="J92" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L92" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
@@ -28974,6 +29013,9 @@
       <c r="J93" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L93" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
@@ -29000,6 +29042,9 @@
       <c r="J94" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L94" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -29026,6 +29071,9 @@
       <c r="J95" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="L95" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
@@ -29052,8 +29100,11 @@
       <c r="J96" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L96" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>296</v>
       </c>
@@ -29078,8 +29129,11 @@
       <c r="J97" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L97" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -29104,8 +29158,11 @@
       <c r="J98" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L98" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>296</v>
       </c>
@@ -29130,8 +29187,11 @@
       <c r="J99" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L99" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>296</v>
       </c>
@@ -29156,8 +29216,11 @@
       <c r="J100" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L100" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>296</v>
       </c>
@@ -29182,8 +29245,11 @@
       <c r="J101" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L101" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>296</v>
       </c>
@@ -29208,8 +29274,11 @@
       <c r="J102" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L102" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>296</v>
       </c>
@@ -29234,8 +29303,11 @@
       <c r="J103" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L103" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>296</v>
       </c>
@@ -29260,8 +29332,11 @@
       <c r="J104" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>296</v>
       </c>
@@ -29286,8 +29361,11 @@
       <c r="J105" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L105" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>296</v>
       </c>
@@ -29312,8 +29390,11 @@
       <c r="J106" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>297</v>
       </c>
@@ -29338,8 +29419,11 @@
       <c r="J107" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L107" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>306</v>
       </c>
@@ -29364,8 +29448,11 @@
       <c r="J108" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>306</v>
       </c>
@@ -29390,8 +29477,11 @@
       <c r="J109" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L109" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>306</v>
       </c>
@@ -29415,6 +29505,9 @@
       </c>
       <c r="J110" s="3" t="s">
         <v>160</v>
+      </c>
+      <c r="L110" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates with left trim = 20
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
+++ b/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE20D25-2DA5-47BB-AAF8-1800C8DBBDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF677E9-7E9A-4D47-9B50-00022D81D832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6065" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6141" uniqueCount="516">
   <si>
     <t>Sequence</t>
   </si>
@@ -9490,6 +9490,18 @@
   </si>
   <si>
     <t>98.09% Xenolumpenus longipterus, Poroclinus rothrocki</t>
+  </si>
+  <si>
+    <t>NOT PLAUSIBLE BY RANGE - according to ADFG</t>
+  </si>
+  <si>
+    <t>Plausible By Range?</t>
+  </si>
+  <si>
+    <t>UNLIKELY BUT POSSIBLE - pee ADFG</t>
+  </si>
+  <si>
+    <t>plausible by range - fishbase</t>
   </si>
 </sst>
 </file>
@@ -9647,7 +9659,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9702,7 +9714,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -10015,12 +10026,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="A293" sqref="A293"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="196.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>
@@ -22191,8 +22203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BCACDE-7C62-4795-BCF1-A029DECBB41A}">
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView topLeftCell="H29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26562,14 +26574,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5085614D-A8E1-47C2-8EAC-787C4920C226}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="12.265625" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -26584,7 +26597,7 @@
     <col min="13" max="13" width="23.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -26624,40 +26637,46 @@
       <c r="M1" s="1" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="29" t="s">
+      <c r="N1" s="27" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="29" t="s">
+      <c r="C2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="28" t="s">
         <v>487</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N2" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>151</v>
       </c>
@@ -26689,7 +26708,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>151</v>
       </c>
@@ -26721,7 +26740,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>151</v>
       </c>
@@ -26753,7 +26772,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>151</v>
       </c>
@@ -26785,7 +26804,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>151</v>
       </c>
@@ -26817,7 +26836,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>151</v>
       </c>
@@ -26849,7 +26868,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>151</v>
       </c>
@@ -26881,7 +26900,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>151</v>
       </c>
@@ -26913,7 +26932,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>152</v>
       </c>
@@ -26945,1383 +26964,1512 @@
         <v>505</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="29" t="s">
+      <c r="C12" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L12" s="29" t="s">
+      <c r="L12" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="29" t="s">
+      <c r="N12" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="29" t="s">
+      <c r="C13" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="28" t="s">
         <v>492</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="29" t="s">
+      <c r="N13" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="29" t="s">
+      <c r="C14" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L14" s="30" t="s">
+      <c r="L14" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="29" t="s">
+      <c r="N14" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="29" t="s">
+      <c r="C15" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="29" t="s">
+      <c r="N15" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="29" t="s">
+      <c r="C16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L16" s="30" t="s">
+      <c r="L16" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="29" t="s">
+      <c r="N16" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="29" t="s">
+      <c r="C17" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="29" t="s">
+      <c r="N17" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="29" t="s">
+      <c r="C18" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L18" s="30" t="s">
+      <c r="L18" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M18" s="29" t="s">
+      <c r="M18" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="29" t="s">
+      <c r="N18" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="29" t="s">
+      <c r="C19" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L19" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="29" t="s">
+      <c r="N19" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="29" t="s">
+      <c r="C20" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="L20" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M20" s="29" t="s">
+      <c r="M20" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="29" t="s">
+      <c r="N20" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="29" t="s">
+      <c r="C21" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L21" s="30" t="s">
+      <c r="L21" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M21" s="29" t="s">
+      <c r="M21" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="29" t="s">
+      <c r="N21" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="29" t="s">
+      <c r="C22" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L22" s="30" t="s">
+      <c r="L22" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M22" s="29" t="s">
+      <c r="M22" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="29" t="s">
+      <c r="N22" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="29" t="s">
+      <c r="C23" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L23" s="30" t="s">
+      <c r="L23" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M23" s="29" t="s">
+      <c r="M23" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="29" t="s">
+      <c r="N23" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="29" t="s">
+      <c r="C24" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M24" s="29" t="s">
+      <c r="M24" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="29" t="s">
+      <c r="N24" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="29" t="s">
+      <c r="C25" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L25" s="30" t="s">
+      <c r="L25" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M25" s="29" t="s">
+      <c r="M25" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="29" t="s">
+      <c r="N25" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="29" t="s">
+      <c r="C26" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L26" s="30" t="s">
+      <c r="L26" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M26" s="29" t="s">
+      <c r="M26" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="29" t="s">
+      <c r="N26" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="29" t="s">
+      <c r="C27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L27" s="30" t="s">
+      <c r="L27" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="29" t="s">
+      <c r="N27" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="29" t="s">
+      <c r="C28" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="29" t="s">
+      <c r="J28" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L28" s="30" t="s">
+      <c r="L28" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M28" s="29" t="s">
+      <c r="M28" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="29" t="s">
+      <c r="N28" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="29" t="s">
+      <c r="C29" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L29" s="30" t="s">
+      <c r="L29" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="29" t="s">
+      <c r="N29" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="29" t="s">
+      <c r="C30" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L30" s="30" t="s">
+      <c r="L30" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="29" t="s">
+      <c r="N30" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="29" t="s">
+      <c r="C31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G31" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L31" s="30" t="s">
+      <c r="L31" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M31" s="29" t="s">
+      <c r="M31" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="29" t="s">
+      <c r="N31" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="29" t="s">
+      <c r="C32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="J32" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L32" s="30" t="s">
+      <c r="L32" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M32" s="29" t="s">
+      <c r="M32" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="29" t="s">
+      <c r="N32" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="29" t="s">
+      <c r="C33" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="G33" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="J33" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L33" s="30" t="s">
+      <c r="L33" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M33" s="29" t="s">
+      <c r="M33" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="29" t="s">
+      <c r="N33" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="29" t="s">
+      <c r="C34" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="29" t="s">
+      <c r="J34" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M34" s="29" t="s">
+      <c r="M34" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="29" t="s">
+      <c r="N34" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="29" t="s">
+      <c r="C35" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="29" t="s">
+      <c r="G35" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J35" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L35" s="30" t="s">
+      <c r="L35" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M35" s="29" t="s">
+      <c r="M35" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="29" t="s">
+      <c r="N35" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="29" t="s">
+      <c r="C36" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="29" t="s">
+      <c r="G36" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J36" s="29" t="s">
+      <c r="J36" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L36" s="30" t="s">
+      <c r="L36" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M36" s="29" t="s">
+      <c r="M36" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="29" t="s">
+      <c r="N36" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="29" t="s">
+      <c r="C37" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="29" t="s">
+      <c r="J37" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L37" s="30" t="s">
+      <c r="L37" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M37" s="29" t="s">
+      <c r="M37" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="29" t="s">
+      <c r="N37" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="29" t="s">
+      <c r="C38" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J38" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L38" s="30" t="s">
+      <c r="L38" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M38" s="29" t="s">
+      <c r="M38" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="29" t="s">
+      <c r="N38" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="29" t="s">
+      <c r="C39" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J39" s="29" t="s">
+      <c r="J39" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L39" s="30" t="s">
+      <c r="L39" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M39" s="29" t="s">
+      <c r="M39" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="29" t="s">
+      <c r="N39" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="29" t="s">
+      <c r="C40" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J40" s="29" t="s">
+      <c r="J40" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M40" s="29" t="s">
+      <c r="M40" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="29" t="s">
+      <c r="N40" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="29" t="s">
+      <c r="C41" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="29" t="s">
+      <c r="G41" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="29" t="s">
+      <c r="J41" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L41" s="30" t="s">
+      <c r="L41" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M41" s="29" t="s">
+      <c r="M41" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="29" t="s">
+      <c r="N41" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="29" t="s">
+      <c r="C42" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="29" t="s">
+      <c r="G42" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J42" s="29" t="s">
+      <c r="J42" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L42" s="30" t="s">
+      <c r="L42" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M42" s="29" t="s">
+      <c r="M42" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="29" t="s">
+      <c r="N42" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="29" t="s">
+      <c r="C43" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J43" s="29" t="s">
+      <c r="J43" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L43" s="30" t="s">
+      <c r="L43" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M43" s="29" t="s">
+      <c r="M43" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="29" t="s">
+      <c r="N43" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="29" t="s">
+      <c r="C44" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J44" s="29" t="s">
+      <c r="J44" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L44" s="30" t="s">
+      <c r="L44" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M44" s="29" t="s">
+      <c r="M44" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="29" t="s">
+      <c r="N44" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="29" t="s">
+      <c r="C45" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="29" t="s">
+      <c r="G45" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J45" s="29" t="s">
+      <c r="J45" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L45" s="30" t="s">
+      <c r="L45" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M45" s="29" t="s">
+      <c r="M45" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="29" t="s">
+      <c r="N45" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="29" t="s">
+      <c r="C46" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G46" s="29" t="s">
+      <c r="G46" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J46" s="29" t="s">
+      <c r="J46" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L46" s="30" t="s">
+      <c r="L46" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M46" s="29" t="s">
+      <c r="M46" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="29" t="s">
+      <c r="N46" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="29" t="s">
+      <c r="C47" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J47" s="29" t="s">
+      <c r="J47" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L47" s="30" t="s">
+      <c r="L47" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M47" s="29" t="s">
+      <c r="M47" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="29" t="s">
+      <c r="N47" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="29" t="s">
+      <c r="C48" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G48" s="29" t="s">
+      <c r="G48" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J48" s="29" t="s">
+      <c r="J48" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L48" s="30" t="s">
+      <c r="L48" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M48" s="29" t="s">
+      <c r="M48" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="29" t="s">
+      <c r="N48" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="29" t="s">
+      <c r="C49" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G49" s="29" t="s">
+      <c r="G49" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J49" s="29" t="s">
+      <c r="J49" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L49" s="30" t="s">
+      <c r="L49" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M49" s="29" t="s">
+      <c r="M49" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="29" t="s">
+      <c r="N49" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F50" s="29" t="s">
+      <c r="C50" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="29" t="s">
+      <c r="G50" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="29" t="s">
+      <c r="J50" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L50" s="30" t="s">
+      <c r="L50" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M50" s="29" t="s">
+      <c r="M50" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="29" t="s">
+      <c r="N50" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="29" t="s">
+      <c r="C51" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J51" s="29" t="s">
+      <c r="J51" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L51" s="30" t="s">
+      <c r="L51" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="M51" s="29" t="s">
+      <c r="M51" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="29" t="s">
+      <c r="N51" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="29" t="s">
+      <c r="C52" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G52" s="29" t="s">
+      <c r="G52" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J52" s="29" t="s">
+      <c r="J52" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L52" s="30" t="s">
+      <c r="L52" s="29" t="s">
         <v>494</v>
       </c>
-      <c r="M52" s="29" t="s">
+      <c r="M52" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="29" t="s">
+      <c r="N52" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="29" t="s">
+      <c r="C53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="G53" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J53" s="29" t="s">
+      <c r="J53" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L53" s="30" t="s">
+      <c r="L53" s="29" t="s">
         <v>495</v>
       </c>
-      <c r="M53" s="29" t="s">
+      <c r="M53" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="29" t="s">
+      <c r="N53" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="29" t="s">
+      <c r="C54" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G54" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J54" s="29" t="s">
+      <c r="J54" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="L54" s="30" t="s">
+      <c r="L54" s="29" t="s">
         <v>495</v>
       </c>
-      <c r="M54" s="29" t="s">
+      <c r="M54" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N54" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>178</v>
       </c>
@@ -28338,1021 +28486,1066 @@
         <v>506</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="28" t="s">
+    <row r="56" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J56" s="28" t="s">
+      <c r="J56" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L56" s="28" t="s">
+      <c r="L56" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="28" t="s">
+    <row r="57" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J57" s="28" t="s">
+      <c r="J57" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L57" s="28" t="s">
+      <c r="L57" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="28" t="s">
+    <row r="58" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J58" s="28" t="s">
+      <c r="J58" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L58" s="28" t="s">
+      <c r="L58" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="28" t="s">
+    <row r="59" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J59" s="28" t="s">
+      <c r="J59" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L59" s="28" t="s">
+      <c r="L59" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="28" t="s">
+    <row r="60" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J60" s="28" t="s">
+      <c r="J60" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L60" s="28" t="s">
+      <c r="L60" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="28" t="s">
+    <row r="61" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J61" s="28" t="s">
+      <c r="J61" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L61" s="28" t="s">
+      <c r="L61" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="28" t="s">
+    <row r="62" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J62" s="28" t="s">
+      <c r="J62" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L62" s="28" t="s">
+      <c r="L62" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="28" t="s">
+    <row r="63" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J63" s="28" t="s">
+      <c r="J63" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L63" s="28" t="s">
+      <c r="L63" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="28" t="s">
+    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J64" s="28" t="s">
+      <c r="J64" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L64" s="28" t="s">
+      <c r="L64" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M64" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="28" t="s">
+    <row r="65" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B65" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J65" s="28" t="s">
+      <c r="J65" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L65" s="28" t="s">
+      <c r="L65" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M65" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="28" t="s">
+    <row r="66" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="28" t="s">
+      <c r="B66" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="28" t="s">
+      <c r="J66" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L66" s="28" t="s">
+      <c r="L66" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M66" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="28" t="s">
+    <row r="67" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J67" s="28" t="s">
+      <c r="J67" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L67" s="28" t="s">
+      <c r="L67" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M67" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="28" t="s">
+    <row r="68" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J68" s="28" t="s">
+      <c r="J68" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L68" s="28" t="s">
+      <c r="L68" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M68" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="28" t="s">
+    <row r="69" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="28" t="s">
+      <c r="B69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J69" s="28" t="s">
+      <c r="J69" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L69" s="28" t="s">
+      <c r="L69" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M69" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="28" t="s">
+    <row r="70" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J70" s="28" t="s">
+      <c r="J70" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L70" s="28" t="s">
+      <c r="L70" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M70" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="28" t="s">
+    <row r="71" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J71" s="28" t="s">
+      <c r="J71" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="L71" s="28" t="s">
+      <c r="L71" s="2" t="s">
         <v>496</v>
       </c>
       <c r="M71" s="4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="31" t="s">
+    <row r="72" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F72" s="31" t="s">
+      <c r="C72" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G72" s="31" t="s">
+      <c r="G72" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="H72" s="31" t="s">
+      <c r="H72" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="J72" s="31" t="s">
+      <c r="J72" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="L72" s="31" t="s">
+      <c r="L72" s="30" t="s">
         <v>497</v>
       </c>
-      <c r="M72" s="29" t="s">
+      <c r="M72" s="28" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="28" t="s">
+    <row r="73" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C73" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F73" s="28" t="s">
+      <c r="C73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="28" t="s">
+      <c r="G73" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J73" s="28" t="s">
+      <c r="J73" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L73" s="28" t="s">
+      <c r="L73" s="2" t="s">
         <v>498</v>
       </c>
       <c r="M73" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="28" t="s">
+    <row r="74" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B74" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F74" s="28" t="s">
+      <c r="C74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G74" s="28" t="s">
+      <c r="G74" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J74" s="28" t="s">
+      <c r="J74" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L74" s="28" t="s">
+      <c r="L74" s="2" t="s">
         <v>498</v>
       </c>
       <c r="M74" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="28" t="s">
+    <row r="75" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75" s="28" t="s">
+      <c r="C75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G75" s="28" t="s">
+      <c r="G75" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J75" s="28" t="s">
+      <c r="J75" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L75" s="28" t="s">
+      <c r="L75" s="2" t="s">
         <v>498</v>
       </c>
       <c r="M75" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="28" t="s">
+    <row r="76" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B76" s="28" t="s">
+      <c r="B76" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C76" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F76" s="28" t="s">
+      <c r="C76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G76" s="28" t="s">
+      <c r="G76" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J76" s="28" t="s">
+      <c r="J76" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L76" s="28" t="s">
+      <c r="L76" s="2" t="s">
         <v>498</v>
       </c>
       <c r="M76" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="28" t="s">
+    <row r="77" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="28" t="s">
+      <c r="C77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G77" s="28" t="s">
+      <c r="G77" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J77" s="28" t="s">
+      <c r="J77" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="L77" s="28" t="s">
+      <c r="L77" s="2" t="s">
         <v>498</v>
       </c>
       <c r="M77" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="31" t="s">
+    <row r="78" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="B78" s="31" t="s">
+      <c r="B78" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C78" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D78" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F78" s="31" t="s">
+      <c r="C78" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="J78" s="31" t="s">
+      <c r="J78" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="L78" s="31" t="s">
+      <c r="L78" s="30" t="s">
         <v>499</v>
       </c>
-      <c r="M78" s="29" t="s">
+      <c r="M78" s="28" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="31" t="s">
+    <row r="79" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="B79" s="31" t="s">
+      <c r="B79" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C79" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="31" t="s">
+      <c r="C79" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G79" s="31" t="s">
+      <c r="G79" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J79" s="31" t="s">
+      <c r="J79" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="L79" s="31" t="s">
+      <c r="L79" s="30" t="s">
         <v>500</v>
       </c>
-      <c r="M79" s="29" t="s">
+      <c r="M79" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="31" t="s">
+      <c r="N79" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="B80" s="31" t="s">
+      <c r="B80" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D80" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="31" t="s">
+      <c r="C80" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G80" s="31" t="s">
+      <c r="G80" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J80" s="31" t="s">
+      <c r="J80" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="L80" s="31" t="s">
+      <c r="L80" s="30" t="s">
         <v>500</v>
       </c>
-      <c r="M80" s="29" t="s">
+      <c r="M80" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="31" t="s">
+      <c r="N80" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="B81" s="31" t="s">
+      <c r="B81" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C81" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D81" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="31" t="s">
+      <c r="C81" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G81" s="31" t="s">
+      <c r="G81" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J81" s="31" t="s">
+      <c r="J81" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="L81" s="31" t="s">
+      <c r="L81" s="30" t="s">
         <v>500</v>
       </c>
-      <c r="M81" s="29" t="s">
+      <c r="M81" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="31" t="s">
+      <c r="N81" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C82" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="31" t="s">
+      <c r="C82" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G82" s="31" t="s">
+      <c r="G82" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J82" s="31" t="s">
+      <c r="J82" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="L82" s="31" t="s">
+      <c r="L82" s="30" t="s">
         <v>500</v>
       </c>
-      <c r="M82" s="29" t="s">
+      <c r="M82" s="28" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="31" t="s">
+      <c r="N82" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="B83" s="31" t="s">
+      <c r="B83" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" s="31" t="s">
+      <c r="C83" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G83" s="31" t="s">
+      <c r="G83" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J83" s="31" t="s">
+      <c r="J83" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="L83" s="31" t="s">
+      <c r="L83" s="30" t="s">
         <v>511</v>
       </c>
-      <c r="M83" s="29" t="s">
+      <c r="M83" s="28" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="31" t="s">
+      <c r="N83" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" s="31" t="s">
+      <c r="C84" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G84" s="31" t="s">
+      <c r="G84" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J84" s="31" t="s">
+      <c r="J84" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="L84" s="31" t="s">
+      <c r="L84" s="30" t="s">
         <v>501</v>
       </c>
-      <c r="M84" s="29" t="s">
+      <c r="M84" s="28" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="31" t="s">
+      <c r="N84" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="B85" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C85" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="31" t="s">
+      <c r="C85" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G85" s="31" t="s">
+      <c r="G85" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J85" s="31" t="s">
+      <c r="J85" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="L85" s="31" t="s">
+      <c r="L85" s="30" t="s">
         <v>501</v>
       </c>
-      <c r="M85" s="29" t="s">
+      <c r="M85" s="28" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="31" t="s">
+      <c r="N85" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="B86" s="31" t="s">
+      <c r="B86" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C86" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D86" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="31" t="s">
+      <c r="C86" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="G86" s="31" t="s">
+      <c r="G86" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="H86" s="31" t="s">
+      <c r="H86" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="J86" s="31" t="s">
+      <c r="J86" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="L86" s="31" t="s">
+      <c r="L86" s="30" t="s">
         <v>502</v>
       </c>
-      <c r="M86" s="29" t="s">
+      <c r="M86" s="28" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="31" t="s">
+      <c r="N86" s="30" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="B87" s="31" t="s">
+      <c r="B87" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C87" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E87" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="31" t="s">
+      <c r="C87" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="G87" s="31" t="s">
+      <c r="G87" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="H87" s="31" t="s">
+      <c r="H87" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="J87" s="32" t="s">
+      <c r="J87" s="31" t="s">
         <v>352</v>
       </c>
-      <c r="L87" s="31" t="s">
+      <c r="L87" s="30" t="s">
         <v>503</v>
       </c>
-      <c r="M87" s="29" t="s">
+      <c r="M87" s="28" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="31" t="s">
+    <row r="88" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A88" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B88" s="31" t="s">
+      <c r="B88" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C88" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F88" s="31" t="s">
+      <c r="C88" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G88" s="31" t="s">
+      <c r="G88" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J88" s="32" t="s">
+      <c r="J88" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L88" s="31" t="s">
+      <c r="L88" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M88" s="31" t="s">
+      <c r="M88" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="31" t="s">
+      <c r="N88" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B89" s="31" t="s">
+      <c r="B89" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F89" s="31" t="s">
+      <c r="C89" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G89" s="31" t="s">
+      <c r="G89" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J89" s="32" t="s">
+      <c r="J89" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L89" s="31" t="s">
+      <c r="L89" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M89" s="31" t="s">
+      <c r="M89" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="31" t="s">
+      <c r="N89" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B90" s="31" t="s">
+      <c r="B90" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F90" s="31" t="s">
+      <c r="C90" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E90" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F90" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G90" s="31" t="s">
+      <c r="G90" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J90" s="32" t="s">
+      <c r="J90" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L90" s="31" t="s">
+      <c r="L90" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M90" s="31" t="s">
+      <c r="M90" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="31" t="s">
+      <c r="N90" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B91" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C91" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="31" t="s">
+      <c r="C91" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G91" s="31" t="s">
+      <c r="G91" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J91" s="32" t="s">
+      <c r="J91" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L91" s="31" t="s">
+      <c r="L91" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M91" s="31" t="s">
+      <c r="M91" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="31" t="s">
+      <c r="N91" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C92" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="31" t="s">
+      <c r="C92" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G92" s="31" t="s">
+      <c r="G92" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J92" s="32" t="s">
+      <c r="J92" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L92" s="31" t="s">
+      <c r="L92" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M92" s="31" t="s">
+      <c r="M92" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="31" t="s">
+      <c r="N92" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B93" s="31" t="s">
+      <c r="B93" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C93" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E93" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F93" s="31" t="s">
+      <c r="C93" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G93" s="31" t="s">
+      <c r="G93" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J93" s="32" t="s">
+      <c r="J93" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L93" s="31" t="s">
+      <c r="L93" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M93" s="31" t="s">
+      <c r="M93" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="31" t="s">
+      <c r="N93" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="B94" s="31" t="s">
+      <c r="B94" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C94" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F94" s="31" t="s">
+      <c r="C94" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="G94" s="31" t="s">
+      <c r="G94" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="J94" s="32" t="s">
+      <c r="J94" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="L94" s="31" t="s">
+      <c r="L94" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="M94" s="31" t="s">
+      <c r="M94" s="30" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N94" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A95" s="19" t="s">
         <v>296</v>
       </c>
@@ -29374,7 +29567,7 @@
       <c r="G95" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J95" s="32" t="s">
+      <c r="J95" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L95" s="19" t="s">
@@ -29383,8 +29576,11 @@
       <c r="M95" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N95" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A96" s="19" t="s">
         <v>296</v>
       </c>
@@ -29406,7 +29602,7 @@
       <c r="G96" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J96" s="32" t="s">
+      <c r="J96" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L96" s="19" t="s">
@@ -29415,8 +29611,11 @@
       <c r="M96" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N96" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A97" s="19" t="s">
         <v>296</v>
       </c>
@@ -29438,7 +29637,7 @@
       <c r="G97" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J97" s="32" t="s">
+      <c r="J97" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L97" s="19" t="s">
@@ -29447,8 +29646,11 @@
       <c r="M97" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N97" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A98" s="19" t="s">
         <v>296</v>
       </c>
@@ -29470,7 +29672,7 @@
       <c r="G98" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J98" s="32" t="s">
+      <c r="J98" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L98" s="19" t="s">
@@ -29479,8 +29681,11 @@
       <c r="M98" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N98" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A99" s="19" t="s">
         <v>296</v>
       </c>
@@ -29502,7 +29707,7 @@
       <c r="G99" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J99" s="32" t="s">
+      <c r="J99" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L99" s="19" t="s">
@@ -29511,8 +29716,11 @@
       <c r="M99" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N99" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A100" s="19" t="s">
         <v>296</v>
       </c>
@@ -29534,7 +29742,7 @@
       <c r="G100" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J100" s="32" t="s">
+      <c r="J100" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L100" s="19" t="s">
@@ -29543,8 +29751,11 @@
       <c r="M100" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N100" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A101" s="19" t="s">
         <v>296</v>
       </c>
@@ -29566,7 +29777,7 @@
       <c r="G101" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J101" s="32" t="s">
+      <c r="J101" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L101" s="19" t="s">
@@ -29575,8 +29786,11 @@
       <c r="M101" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N101" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A102" s="19" t="s">
         <v>296</v>
       </c>
@@ -29598,7 +29812,7 @@
       <c r="G102" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J102" s="32" t="s">
+      <c r="J102" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L102" s="19" t="s">
@@ -29607,8 +29821,11 @@
       <c r="M102" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N102" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A103" s="19" t="s">
         <v>296</v>
       </c>
@@ -29630,7 +29847,7 @@
       <c r="G103" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J103" s="32" t="s">
+      <c r="J103" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L103" s="19" t="s">
@@ -29639,8 +29856,11 @@
       <c r="M103" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N103" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A104" s="19" t="s">
         <v>296</v>
       </c>
@@ -29662,7 +29882,7 @@
       <c r="G104" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J104" s="32" t="s">
+      <c r="J104" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L104" s="19" t="s">
@@ -29671,8 +29891,11 @@
       <c r="M104" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N104" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A105" s="19" t="s">
         <v>296</v>
       </c>
@@ -29694,7 +29917,7 @@
       <c r="G105" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J105" s="32" t="s">
+      <c r="J105" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L105" s="19" t="s">
@@ -29703,8 +29926,11 @@
       <c r="M105" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N105" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="19" t="s">
         <v>296</v>
       </c>
@@ -29726,7 +29952,7 @@
       <c r="G106" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J106" s="32" t="s">
+      <c r="J106" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L106" s="19" t="s">
@@ -29735,8 +29961,11 @@
       <c r="M106" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N106" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A107" s="19" t="s">
         <v>297</v>
       </c>
@@ -29758,7 +29987,7 @@
       <c r="G107" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="J107" s="32" t="s">
+      <c r="J107" s="31" t="s">
         <v>308</v>
       </c>
       <c r="L107" s="19" t="s">
@@ -29767,8 +29996,11 @@
       <c r="M107" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N107" s="28" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A108" s="19" t="s">
         <v>306</v>
       </c>
@@ -29790,7 +30022,7 @@
       <c r="G108" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J108" s="32" t="s">
+      <c r="J108" s="31" t="s">
         <v>160</v>
       </c>
       <c r="L108" s="19" t="s">
@@ -29799,8 +30031,11 @@
       <c r="M108" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N108" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A109" s="19" t="s">
         <v>306</v>
       </c>
@@ -29822,7 +30057,7 @@
       <c r="G109" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J109" s="32" t="s">
+      <c r="J109" s="31" t="s">
         <v>160</v>
       </c>
       <c r="L109" s="19" t="s">
@@ -29831,8 +30066,11 @@
       <c r="M109" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N109" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A110" s="19" t="s">
         <v>306</v>
       </c>
@@ -29854,7 +30092,7 @@
       <c r="G110" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J110" s="32" t="s">
+      <c r="J110" s="31" t="s">
         <v>160</v>
       </c>
       <c r="L110" s="19" t="s">
@@ -29862,6 +30100,9 @@
       </c>
       <c r="M110" s="19" t="s">
         <v>504</v>
+      </c>
+      <c r="N110" s="28" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
organizes files; gets rid of old versions. Updates towards fixing binomial species assignment issue
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
+++ b/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9EF677E9-7E9A-4D47-9B50-00022D81D832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC75794-1029-4149-94EB-041F27D8C372}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped" sheetId="1" r:id="rId1"/>
@@ -9735,6 +9735,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10026,8 +10030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18024,8 +18028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF18E0B1-8AFD-4421-A418-DA9540F90652}">
   <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22203,8 +22207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BCACDE-7C62-4795-BCF1-A029DECBB41A}">
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26577,7 +26581,7 @@
   <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates with work on addpecies function
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
+++ b/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9EF677E9-7E9A-4D47-9B50-00022D81D832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC75794-1029-4149-94EB-041F27D8C372}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="Unresolved (2)" sheetId="4" r:id="rId3"/>
     <sheet name="Unassigned" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -10030,8 +10043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A189" sqref="A189"/>
+    <sheetView topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A334" sqref="A334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18028,8 +18041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF18E0B1-8AFD-4421-A418-DA9540F90652}">
   <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22207,8 +22220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BCACDE-7C62-4795-BCF1-A029DECBB41A}">
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K82" sqref="K82"/>
+    <sheetView topLeftCell="I64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Addresses addSpecies issues (DOES NOT FIX) - created a merged table to compare across taxonomy assignment methods
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
+++ b/Deliverables/Copy of Copy of WADE003-arcticpred-12SP1-taxa-mapped_1 AB_JP (version 1).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9EF677E9-7E9A-4D47-9B50-00022D81D832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC75794-1029-4149-94EB-041F27D8C372}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="Unresolved (2)" sheetId="4" r:id="rId3"/>
     <sheet name="Unassigned" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -9735,6 +9748,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10026,8 +10043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A334" sqref="A334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18024,8 +18041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF18E0B1-8AFD-4421-A418-DA9540F90652}">
   <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22203,8 +22220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45BCACDE-7C62-4795-BCF1-A029DECBB41A}">
   <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView topLeftCell="I64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26577,7 +26594,7 @@
   <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>